<commit_message>
updated federal, state, sub-state changes through Dec 31 2018
</commit_message>
<xml_diff>
--- a/rawdata/FederalMinimumWage_Changes.xlsx
+++ b/rawdata/FederalMinimumWage_Changes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -185,20 +185,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:16"/>
+  <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.63775510204082"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.64"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -460,13 +460,13 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>7.25</v>
@@ -478,7 +478,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>